<commit_message>
test and fix issues - more work need to fix
Former-commit-id: 1d00b5662b25b6f297814eb38b8624427a2d72cb
</commit_message>
<xml_diff>
--- a/excel_templates/tenant-template.xlsx
+++ b/excel_templates/tenant-template.xlsx
@@ -61,6 +61,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -123,6 +126,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -408,7 +414,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +465,7 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="D2" s="5"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -473,7 +479,7 @@
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="5"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -487,7 +493,7 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="5"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -501,7 +507,7 @@
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="5"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -515,7 +521,7 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -529,7 +535,7 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="5"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -543,7 +549,7 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="5"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -557,7 +563,7 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -571,7 +577,7 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -585,7 +591,7 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -599,7 +605,7 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -613,7 +619,7 @@
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -627,7 +633,7 @@
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -641,7 +647,7 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -655,7 +661,7 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="D16" s="5"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -669,7 +675,7 @@
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="D17" s="5"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -683,7 +689,7 @@
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -697,7 +703,7 @@
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -711,7 +717,7 @@
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="D20" s="5"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -725,7 +731,7 @@
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="D21" s="5"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -739,7 +745,7 @@
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -753,7 +759,7 @@
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -767,7 +773,7 @@
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -781,7 +787,7 @@
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>

</xml_diff>

<commit_message>
do the hot fix separation and modify the template for leaseargm
</commit_message>
<xml_diff>
--- a/excel_templates/tenant-template.xlsx
+++ b/excel_templates/tenant-template.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
   <si>
     <t>Company Name</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>PKK</t>
+  </si>
+  <si>
+    <t>Separate</t>
   </si>
 </sst>
 </file>
@@ -724,12 +727,12 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A6" sqref="A6:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
@@ -972,7 +975,9 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>

</xml_diff>